<commit_message>
Add final future cut
</commit_message>
<xml_diff>
--- a/TEEmployee/App_Data/user-以群組、小組、身分分類v4.xlsx
+++ b/TEEmployee/App_Data/user-以群組、小組、身分分類v4.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\NETCORE\TEEmployee\TEEmployee\App_Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="510" yWindow="600" windowWidth="24240" windowHeight="11505"/>
   </bookViews>
@@ -10,12 +15,12 @@
     <sheet name="計畫主管以重要主管分類" sheetId="2" r:id="rId1"/>
     <sheet name="計畫主管以計畫編號分類" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1800" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1801" uniqueCount="474">
   <si>
     <t>empno</t>
   </si>
@@ -1564,8 +1569,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="13">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -2012,18 +2017,6 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2052,6 +2045,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2114,7 +2119,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2146,9 +2151,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2180,6 +2186,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2355,20 +2362,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:AH84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A48" sqref="A48:XFD48"/>
+      <selection pane="bottomRight" activeCell="N82" sqref="N82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="31.140625" customWidth="1"/>
     <col min="9" max="11" width="11.7109375" style="21" customWidth="1"/>
@@ -2391,7 +2398,7 @@
     <col min="33" max="33" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2449,7 +2456,7 @@
       <c r="S1" s="27"/>
       <c r="T1" s="27"/>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>170</v>
       </c>
@@ -2497,7 +2504,7 @@
       </c>
       <c r="T2" s="27"/>
     </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>281</v>
       </c>
@@ -2546,16 +2553,16 @@
       <c r="U3" s="21"/>
       <c r="V3" s="21"/>
       <c r="W3" s="21"/>
-      <c r="X3" s="54" t="str">
+      <c r="X3" s="64" t="str">
         <f>I1</f>
         <v>部門主管</v>
       </c>
-      <c r="Y3" s="55"/>
+      <c r="Y3" s="65"/>
       <c r="Z3" s="21"/>
       <c r="AA3" s="21"/>
       <c r="AB3" s="21"/>
     </row>
-    <row r="4" spans="1:34">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>110</v>
       </c>
@@ -2612,7 +2619,7 @@
       <c r="AA4" s="21"/>
       <c r="AB4" s="21"/>
     </row>
-    <row r="5" spans="1:34">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>117</v>
       </c>
@@ -2661,7 +2668,7 @@
       <c r="AA5" s="21"/>
       <c r="AB5" s="21"/>
     </row>
-    <row r="6" spans="1:34">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>337</v>
       </c>
@@ -2716,7 +2723,7 @@
       <c r="AG6" s="31"/>
       <c r="AH6" s="32"/>
     </row>
-    <row r="7" spans="1:34">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>289</v>
       </c>
@@ -2756,24 +2763,24 @@
       <c r="Q7" s="17"/>
       <c r="R7" s="17"/>
       <c r="S7" s="7"/>
-      <c r="U7" s="58" t="s">
+      <c r="U7" s="54" t="s">
         <v>443</v>
       </c>
-      <c r="V7" s="59"/>
+      <c r="V7" s="55"/>
       <c r="W7" s="21"/>
-      <c r="X7" s="60" t="s">
+      <c r="X7" s="56" t="s">
         <v>444</v>
       </c>
-      <c r="Y7" s="60"/>
+      <c r="Y7" s="56"/>
       <c r="Z7" s="21"/>
-      <c r="AA7" s="61" t="s">
+      <c r="AA7" s="57" t="s">
         <v>445</v>
       </c>
-      <c r="AB7" s="61"/>
+      <c r="AB7" s="57"/>
       <c r="AE7" s="32"/>
       <c r="AH7" s="32"/>
     </row>
-    <row r="8" spans="1:34">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>98</v>
       </c>
@@ -2841,7 +2848,7 @@
       <c r="AE8" s="33"/>
       <c r="AH8" s="33"/>
     </row>
-    <row r="9" spans="1:34">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="38">
         <v>8056</v>
       </c>
@@ -2881,28 +2888,28 @@
       <c r="Q9" s="17"/>
       <c r="R9" s="17"/>
       <c r="S9" s="7"/>
-      <c r="U9" s="62" t="s">
+      <c r="U9" s="58" t="s">
         <v>439</v>
       </c>
-      <c r="V9" s="63"/>
-      <c r="X9" s="64" t="s">
+      <c r="V9" s="59"/>
+      <c r="X9" s="60" t="s">
         <v>439</v>
       </c>
-      <c r="Y9" s="65"/>
-      <c r="AA9" s="66" t="s">
+      <c r="Y9" s="61"/>
+      <c r="AA9" s="62" t="s">
         <v>439</v>
       </c>
-      <c r="AB9" s="67"/>
-      <c r="AD9" s="56" t="s">
+      <c r="AB9" s="63"/>
+      <c r="AD9" s="66" t="s">
         <v>442</v>
       </c>
-      <c r="AE9" s="56"/>
-      <c r="AG9" s="56" t="s">
+      <c r="AE9" s="66"/>
+      <c r="AG9" s="66" t="s">
         <v>439</v>
       </c>
-      <c r="AH9" s="56"/>
-    </row>
-    <row r="10" spans="1:34">
+      <c r="AH9" s="66"/>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>62</v>
       </c>
@@ -2968,12 +2975,12 @@
       <c r="AE10" s="5" t="s">
         <v>458</v>
       </c>
-      <c r="AG10" s="57" t="s">
+      <c r="AG10" s="67" t="s">
         <v>440</v>
       </c>
-      <c r="AH10" s="57"/>
-    </row>
-    <row r="11" spans="1:34">
+      <c r="AH10" s="67"/>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -3041,12 +3048,12 @@
       <c r="AE11" s="5" t="s">
         <v>446</v>
       </c>
-      <c r="AG11" s="57" t="s">
+      <c r="AG11" s="67" t="s">
         <v>441</v>
       </c>
-      <c r="AH11" s="57"/>
-    </row>
-    <row r="12" spans="1:34">
+      <c r="AH11" s="67"/>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>273</v>
       </c>
@@ -3111,7 +3118,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="13" spans="1:34">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>221</v>
       </c>
@@ -3152,7 +3159,7 @@
       <c r="R13" s="17"/>
       <c r="S13" s="7"/>
     </row>
-    <row r="14" spans="1:34">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>269</v>
       </c>
@@ -3195,7 +3202,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="15" spans="1:34">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>333</v>
       </c>
@@ -3236,7 +3243,7 @@
       <c r="R15" s="17"/>
       <c r="S15" s="7"/>
     </row>
-    <row r="16" spans="1:34">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>58</v>
       </c>
@@ -3279,7 +3286,7 @@
       <c r="R16" s="17"/>
       <c r="S16" s="7"/>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>70</v>
       </c>
@@ -3320,7 +3327,7 @@
       <c r="R17" s="17"/>
       <c r="S17" s="7"/>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>265</v>
       </c>
@@ -3361,7 +3368,7 @@
       <c r="R18" s="17"/>
       <c r="S18" s="7"/>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>90</v>
       </c>
@@ -3402,7 +3409,7 @@
       <c r="R19" s="17"/>
       <c r="S19" s="7"/>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>102</v>
       </c>
@@ -3443,7 +3450,7 @@
       <c r="R20" s="17"/>
       <c r="S20" s="7"/>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>249</v>
       </c>
@@ -3490,7 +3497,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>174</v>
       </c>
@@ -3535,7 +3542,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="38">
         <v>7458</v>
       </c>
@@ -3576,7 +3583,7 @@
       <c r="R23" s="17"/>
       <c r="S23" s="7"/>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>321</v>
       </c>
@@ -3625,7 +3632,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>41</v>
       </c>
@@ -3672,7 +3679,7 @@
       <c r="R25" s="16"/>
       <c r="S25" s="7"/>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>318</v>
       </c>
@@ -3713,7 +3720,7 @@
       <c r="R26" s="16"/>
       <c r="S26" s="7"/>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>166</v>
       </c>
@@ -3754,7 +3761,7 @@
       <c r="R27" s="16"/>
       <c r="S27" s="7"/>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>285</v>
       </c>
@@ -3795,7 +3802,7 @@
       <c r="R28" s="16"/>
       <c r="S28" s="7"/>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>253</v>
       </c>
@@ -3837,7 +3844,7 @@
       <c r="S29" s="7"/>
       <c r="T29" s="8"/>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>257</v>
       </c>
@@ -3878,7 +3885,7 @@
       <c r="R30" s="16"/>
       <c r="S30" s="7"/>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>74</v>
       </c>
@@ -3919,7 +3926,7 @@
       <c r="R31" s="16"/>
       <c r="S31" s="7"/>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>45</v>
       </c>
@@ -3962,7 +3969,7 @@
       <c r="R32" s="16"/>
       <c r="S32" s="7"/>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>78</v>
       </c>
@@ -4003,7 +4010,7 @@
       <c r="R33" s="16"/>
       <c r="S33" s="7"/>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>82</v>
       </c>
@@ -4044,7 +4051,7 @@
       <c r="R34" s="16"/>
       <c r="S34" s="7"/>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>106</v>
       </c>
@@ -4087,7 +4094,7 @@
       <c r="R35" s="16"/>
       <c r="S35" s="7"/>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>297</v>
       </c>
@@ -4132,7 +4139,7 @@
       <c r="R36" s="16"/>
       <c r="S36" s="7"/>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>54</v>
       </c>
@@ -4175,7 +4182,7 @@
       <c r="R37" s="16"/>
       <c r="S37" s="7"/>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>86</v>
       </c>
@@ -4218,7 +4225,7 @@
       <c r="R38" s="16"/>
       <c r="S38" s="7"/>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>229</v>
       </c>
@@ -4259,7 +4266,7 @@
       <c r="R39" s="16"/>
       <c r="S39" s="7"/>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>137</v>
       </c>
@@ -4300,7 +4307,7 @@
       <c r="R40" s="16"/>
       <c r="S40" s="7"/>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>146</v>
       </c>
@@ -4341,7 +4348,7 @@
       <c r="R41" s="16"/>
       <c r="S41" s="7"/>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>329</v>
       </c>
@@ -4388,7 +4395,7 @@
       <c r="R42" s="16"/>
       <c r="S42" s="7"/>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>8</v>
       </c>
@@ -4431,7 +4438,7 @@
       <c r="R43" s="16"/>
       <c r="S43" s="7"/>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>37</v>
       </c>
@@ -4474,7 +4481,7 @@
       <c r="R44" s="16"/>
       <c r="S44" s="7"/>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>150</v>
       </c>
@@ -4515,7 +4522,7 @@
       <c r="R45" s="16"/>
       <c r="S45" s="7"/>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>233</v>
       </c>
@@ -4557,7 +4564,7 @@
       <c r="S46" s="7"/>
       <c r="T46" s="8"/>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="50">
         <v>8103</v>
       </c>
@@ -4599,7 +4606,7 @@
       <c r="S47" s="7"/>
       <c r="T47" s="8"/>
     </row>
-    <row r="48" spans="1:20">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="46">
         <v>7340</v>
       </c>
@@ -4641,7 +4648,7 @@
       <c r="S48" s="7"/>
       <c r="T48" s="8"/>
     </row>
-    <row r="49" spans="1:19">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>154</v>
       </c>
@@ -4686,7 +4693,7 @@
       </c>
       <c r="S49" s="7"/>
     </row>
-    <row r="50" spans="1:19">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>133</v>
       </c>
@@ -4733,7 +4740,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="51" spans="1:19">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>121</v>
       </c>
@@ -4774,7 +4781,7 @@
       <c r="R51" s="18"/>
       <c r="S51" s="7"/>
     </row>
-    <row r="52" spans="1:19">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>325</v>
       </c>
@@ -4815,7 +4822,7 @@
       <c r="R52" s="18"/>
       <c r="S52" s="7"/>
     </row>
-    <row r="53" spans="1:19">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>15</v>
       </c>
@@ -4856,7 +4863,7 @@
       <c r="R53" s="18"/>
       <c r="S53" s="7"/>
     </row>
-    <row r="54" spans="1:19">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>33</v>
       </c>
@@ -4897,7 +4904,7 @@
       <c r="R54" s="18"/>
       <c r="S54" s="7"/>
     </row>
-    <row r="55" spans="1:19">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>314</v>
       </c>
@@ -4938,7 +4945,7 @@
       <c r="R55" s="18"/>
       <c r="S55" s="7"/>
     </row>
-    <row r="56" spans="1:19">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>241</v>
       </c>
@@ -4981,7 +4988,7 @@
       <c r="R56" s="18"/>
       <c r="S56" s="7"/>
     </row>
-    <row r="57" spans="1:19">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>189</v>
       </c>
@@ -5022,7 +5029,7 @@
       <c r="R57" s="18"/>
       <c r="S57" s="7"/>
     </row>
-    <row r="58" spans="1:19">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>237</v>
       </c>
@@ -5063,7 +5070,7 @@
       <c r="R58" s="18"/>
       <c r="S58" s="7"/>
     </row>
-    <row r="59" spans="1:19">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>306</v>
       </c>
@@ -5104,7 +5111,7 @@
       <c r="R59" s="18"/>
       <c r="S59" s="7"/>
     </row>
-    <row r="60" spans="1:19">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>29</v>
       </c>
@@ -5145,7 +5152,7 @@
       <c r="R60" s="18"/>
       <c r="S60" s="7"/>
     </row>
-    <row r="61" spans="1:19">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>94</v>
       </c>
@@ -5186,7 +5193,7 @@
       <c r="R61" s="18"/>
       <c r="S61" s="7"/>
     </row>
-    <row r="62" spans="1:19">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="40">
         <v>8026</v>
       </c>
@@ -5227,7 +5234,7 @@
       <c r="R62" s="18"/>
       <c r="S62" s="7"/>
     </row>
-    <row r="63" spans="1:19">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>129</v>
       </c>
@@ -5272,7 +5279,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="64" spans="1:19">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>293</v>
       </c>
@@ -5317,7 +5324,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="65" spans="1:19">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>261</v>
       </c>
@@ -5358,7 +5365,7 @@
       <c r="R65" s="18"/>
       <c r="S65" s="7"/>
     </row>
-    <row r="66" spans="1:19">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>186</v>
       </c>
@@ -5399,7 +5406,7 @@
       <c r="R66" s="18"/>
       <c r="S66" s="7"/>
     </row>
-    <row r="67" spans="1:19">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>125</v>
       </c>
@@ -5440,7 +5447,7 @@
       <c r="R67" s="18"/>
       <c r="S67" s="7"/>
     </row>
-    <row r="68" spans="1:19">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>142</v>
       </c>
@@ -5481,7 +5488,7 @@
       <c r="R68" s="18"/>
       <c r="S68" s="7"/>
     </row>
-    <row r="69" spans="1:19">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>302</v>
       </c>
@@ -5522,7 +5529,7 @@
       <c r="R69" s="18"/>
       <c r="S69" s="7"/>
     </row>
-    <row r="70" spans="1:19">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>341</v>
       </c>
@@ -5563,7 +5570,7 @@
       <c r="R70" s="18"/>
       <c r="S70" s="7"/>
     </row>
-    <row r="71" spans="1:19">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>50</v>
       </c>
@@ -5604,7 +5611,7 @@
       <c r="R71" s="18"/>
       <c r="S71" s="7"/>
     </row>
-    <row r="72" spans="1:19">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>310</v>
       </c>
@@ -5645,7 +5652,7 @@
       <c r="R72" s="18"/>
       <c r="S72" s="7"/>
     </row>
-    <row r="73" spans="1:19">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>216</v>
       </c>
@@ -5686,7 +5693,7 @@
       <c r="R73" s="18"/>
       <c r="S73" s="7"/>
     </row>
-    <row r="74" spans="1:19">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>245</v>
       </c>
@@ -5731,7 +5738,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="75" spans="1:19">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>193</v>
       </c>
@@ -5776,7 +5783,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="76" spans="1:19">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>178</v>
       </c>
@@ -5821,7 +5828,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="77" spans="1:19">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>24</v>
       </c>
@@ -5866,7 +5873,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="78" spans="1:19">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>197</v>
       </c>
@@ -5907,7 +5914,7 @@
       <c r="R78" s="20"/>
       <c r="S78" s="7"/>
     </row>
-    <row r="79" spans="1:19">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>161</v>
       </c>
@@ -5948,7 +5955,7 @@
       <c r="R79" s="20"/>
       <c r="S79" s="7"/>
     </row>
-    <row r="80" spans="1:19">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>182</v>
       </c>
@@ -5989,7 +5996,7 @@
       <c r="R80" s="20"/>
       <c r="S80" s="7"/>
     </row>
-    <row r="81" spans="1:19">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>201</v>
       </c>
@@ -6030,7 +6037,7 @@
       <c r="R81" s="20"/>
       <c r="S81" s="7"/>
     </row>
-    <row r="82" spans="1:19">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>19</v>
       </c>
@@ -6064,14 +6071,16 @@
         <v>361</v>
       </c>
       <c r="M82" s="20"/>
-      <c r="N82" s="20"/>
+      <c r="N82" s="44" t="s">
+        <v>442</v>
+      </c>
       <c r="O82" s="20"/>
       <c r="P82" s="35"/>
       <c r="Q82" s="35"/>
       <c r="R82" s="20"/>
       <c r="S82" s="7"/>
     </row>
-    <row r="83" spans="1:19">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>225</v>
       </c>
@@ -6112,7 +6121,7 @@
       <c r="R83" s="20"/>
       <c r="S83" s="7"/>
     </row>
-    <row r="84" spans="1:19">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>205</v>
       </c>
@@ -6155,17 +6164,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="AG9:AH9"/>
+    <mergeCell ref="AD9:AE9"/>
+    <mergeCell ref="AG10:AH10"/>
+    <mergeCell ref="AG11:AH11"/>
     <mergeCell ref="U7:V7"/>
     <mergeCell ref="X7:Y7"/>
     <mergeCell ref="AA7:AB7"/>
     <mergeCell ref="U9:V9"/>
     <mergeCell ref="X9:Y9"/>
     <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="AG9:AH9"/>
-    <mergeCell ref="AD9:AE9"/>
-    <mergeCell ref="AG10:AH10"/>
-    <mergeCell ref="AG11:AH11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -6183,7 +6192,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U86"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -6193,7 +6202,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="31.140625" customWidth="1"/>
     <col min="9" max="11" width="11.7109375" style="21" customWidth="1"/>
@@ -6201,7 +6210,7 @@
     <col min="13" max="18" width="11.7109375" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -6257,7 +6266,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>321</v>
       </c>
@@ -6302,7 +6311,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>166</v>
       </c>
@@ -6343,7 +6352,7 @@
       <c r="R3" s="16"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>285</v>
       </c>
@@ -6384,7 +6393,7 @@
       <c r="R4" s="16"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>253</v>
       </c>
@@ -6425,7 +6434,7 @@
       <c r="R5" s="16"/>
       <c r="S5" s="7"/>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>257</v>
       </c>
@@ -6466,7 +6475,7 @@
       <c r="R6" s="16"/>
       <c r="S6" s="7"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -6512,7 +6521,7 @@
       <c r="S7" s="14"/>
       <c r="T7" s="8"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>318</v>
       </c>
@@ -6553,7 +6562,7 @@
       <c r="R8" s="16"/>
       <c r="S8" s="7"/>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>74</v>
       </c>
@@ -6594,7 +6603,7 @@
       <c r="R9" s="16"/>
       <c r="S9" s="7"/>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>45</v>
       </c>
@@ -6637,7 +6646,7 @@
       <c r="R10" s="16"/>
       <c r="S10" s="7"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>78</v>
       </c>
@@ -6678,7 +6687,7 @@
       <c r="R11" s="16"/>
       <c r="S11" s="7"/>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>82</v>
       </c>
@@ -6719,7 +6728,7 @@
       <c r="R12" s="16"/>
       <c r="S12" s="7"/>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>106</v>
       </c>
@@ -6760,7 +6769,7 @@
       <c r="R13" s="16"/>
       <c r="S13" s="7"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>297</v>
       </c>
@@ -6805,7 +6814,7 @@
       <c r="R14" s="16"/>
       <c r="S14" s="7"/>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>54</v>
       </c>
@@ -6848,7 +6857,7 @@
       <c r="R15" s="16"/>
       <c r="S15" s="7"/>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>86</v>
       </c>
@@ -6891,7 +6900,7 @@
       <c r="R16" s="16"/>
       <c r="S16" s="7"/>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>229</v>
       </c>
@@ -6932,7 +6941,7 @@
       <c r="R17" s="16"/>
       <c r="S17" s="7"/>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>137</v>
       </c>
@@ -6973,7 +6982,7 @@
       <c r="R18" s="16"/>
       <c r="S18" s="7"/>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>146</v>
       </c>
@@ -7014,7 +7023,7 @@
       <c r="R19" s="16"/>
       <c r="S19" s="7"/>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>329</v>
       </c>
@@ -7061,7 +7070,7 @@
       <c r="R20" s="16"/>
       <c r="S20" s="7"/>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
@@ -7104,7 +7113,7 @@
       <c r="R21" s="16"/>
       <c r="S21" s="7"/>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
@@ -7147,7 +7156,7 @@
       <c r="R22" s="16"/>
       <c r="S22" s="7"/>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>150</v>
       </c>
@@ -7188,7 +7197,7 @@
       <c r="R23" s="16"/>
       <c r="S23" s="7"/>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>233</v>
       </c>
@@ -7229,7 +7238,7 @@
       <c r="R24" s="16"/>
       <c r="S24" s="7"/>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>281</v>
       </c>
@@ -7276,7 +7285,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>110</v>
       </c>
@@ -7321,7 +7330,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>117</v>
       </c>
@@ -7362,7 +7371,7 @@
       <c r="R27" s="17"/>
       <c r="S27" s="7"/>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>337</v>
       </c>
@@ -7403,7 +7412,7 @@
       <c r="R28" s="17"/>
       <c r="S28" s="7"/>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>289</v>
       </c>
@@ -7444,7 +7453,7 @@
       <c r="R29" s="17"/>
       <c r="S29" s="7"/>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>98</v>
       </c>
@@ -7485,7 +7494,7 @@
       <c r="R30" s="17"/>
       <c r="S30" s="7"/>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>62</v>
       </c>
@@ -7528,7 +7537,7 @@
       <c r="R31" s="17"/>
       <c r="S31" s="7"/>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>66</v>
       </c>
@@ -7571,7 +7580,7 @@
       <c r="R32" s="17"/>
       <c r="S32" s="7"/>
     </row>
-    <row r="33" spans="1:21">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>273</v>
       </c>
@@ -7614,7 +7623,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>221</v>
       </c>
@@ -7655,7 +7664,7 @@
       <c r="R34" s="17"/>
       <c r="S34" s="7"/>
     </row>
-    <row r="35" spans="1:21">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>269</v>
       </c>
@@ -7700,7 +7709,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="36" spans="1:21">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>333</v>
       </c>
@@ -7741,7 +7750,7 @@
       <c r="R36" s="17"/>
       <c r="S36" s="7"/>
     </row>
-    <row r="37" spans="1:21">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>58</v>
       </c>
@@ -7784,7 +7793,7 @@
       <c r="R37" s="17"/>
       <c r="S37" s="7"/>
     </row>
-    <row r="38" spans="1:21">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>70</v>
       </c>
@@ -7825,7 +7834,7 @@
       <c r="R38" s="17"/>
       <c r="S38" s="7"/>
     </row>
-    <row r="39" spans="1:21">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>265</v>
       </c>
@@ -7866,7 +7875,7 @@
       <c r="R39" s="17"/>
       <c r="S39" s="7"/>
     </row>
-    <row r="40" spans="1:21">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>90</v>
       </c>
@@ -7907,7 +7916,7 @@
       <c r="R40" s="17"/>
       <c r="S40" s="7"/>
     </row>
-    <row r="41" spans="1:21">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>102</v>
       </c>
@@ -7948,7 +7957,7 @@
       <c r="R41" s="17"/>
       <c r="S41" s="7"/>
     </row>
-    <row r="42" spans="1:21">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>174</v>
       </c>
@@ -7997,7 +8006,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="43" spans="1:21">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>249</v>
       </c>
@@ -8044,7 +8053,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="44" spans="1:21">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>154</v>
       </c>
@@ -8087,7 +8096,7 @@
       <c r="R44" s="26"/>
       <c r="S44" s="7"/>
     </row>
-    <row r="45" spans="1:21">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>133</v>
       </c>
@@ -8136,7 +8145,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="46" spans="1:21">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>277</v>
       </c>
@@ -8182,7 +8191,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="47" spans="1:21">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>261</v>
       </c>
@@ -8223,7 +8232,7 @@
       <c r="R47" s="18"/>
       <c r="S47" s="7"/>
     </row>
-    <row r="48" spans="1:21">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>186</v>
       </c>
@@ -8264,7 +8273,7 @@
       <c r="R48" s="18"/>
       <c r="S48" s="7"/>
     </row>
-    <row r="49" spans="1:19">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>121</v>
       </c>
@@ -8305,7 +8314,7 @@
       <c r="R49" s="18"/>
       <c r="S49" s="7"/>
     </row>
-    <row r="50" spans="1:19">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>325</v>
       </c>
@@ -8346,7 +8355,7 @@
       <c r="R50" s="18"/>
       <c r="S50" s="7"/>
     </row>
-    <row r="51" spans="1:19">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>15</v>
       </c>
@@ -8387,7 +8396,7 @@
       <c r="R51" s="18"/>
       <c r="S51" s="7"/>
     </row>
-    <row r="52" spans="1:19">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>33</v>
       </c>
@@ -8428,7 +8437,7 @@
       <c r="R52" s="18"/>
       <c r="S52" s="7"/>
     </row>
-    <row r="53" spans="1:19">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>50</v>
       </c>
@@ -8469,7 +8478,7 @@
       <c r="R53" s="18"/>
       <c r="S53" s="7"/>
     </row>
-    <row r="54" spans="1:19">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>314</v>
       </c>
@@ -8510,7 +8519,7 @@
       <c r="R54" s="18"/>
       <c r="S54" s="7"/>
     </row>
-    <row r="55" spans="1:19">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>241</v>
       </c>
@@ -8553,7 +8562,7 @@
       <c r="R55" s="18"/>
       <c r="S55" s="7"/>
     </row>
-    <row r="56" spans="1:19">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>189</v>
       </c>
@@ -8594,7 +8603,7 @@
       <c r="R56" s="18"/>
       <c r="S56" s="7"/>
     </row>
-    <row r="57" spans="1:19">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>237</v>
       </c>
@@ -8635,7 +8644,7 @@
       <c r="R57" s="18"/>
       <c r="S57" s="7"/>
     </row>
-    <row r="58" spans="1:19">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>306</v>
       </c>
@@ -8676,7 +8685,7 @@
       <c r="R58" s="18"/>
       <c r="S58" s="7"/>
     </row>
-    <row r="59" spans="1:19">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>29</v>
       </c>
@@ -8717,7 +8726,7 @@
       <c r="R59" s="18"/>
       <c r="S59" s="7"/>
     </row>
-    <row r="60" spans="1:19">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>94</v>
       </c>
@@ -8758,7 +8767,7 @@
       <c r="R60" s="18"/>
       <c r="S60" s="7"/>
     </row>
-    <row r="61" spans="1:19">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>129</v>
       </c>
@@ -8803,7 +8812,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="62" spans="1:19">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>293</v>
       </c>
@@ -8848,7 +8857,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="63" spans="1:19">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>125</v>
       </c>
@@ -8889,7 +8898,7 @@
       <c r="R63" s="18"/>
       <c r="S63" s="7"/>
     </row>
-    <row r="64" spans="1:19">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>142</v>
       </c>
@@ -8930,7 +8939,7 @@
       <c r="R64" s="18"/>
       <c r="S64" s="7"/>
     </row>
-    <row r="65" spans="1:19">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>302</v>
       </c>
@@ -8971,7 +8980,7 @@
       <c r="R65" s="18"/>
       <c r="S65" s="7"/>
     </row>
-    <row r="66" spans="1:19">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>341</v>
       </c>
@@ -9012,7 +9021,7 @@
       <c r="R66" s="18"/>
       <c r="S66" s="7"/>
     </row>
-    <row r="67" spans="1:19">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>310</v>
       </c>
@@ -9053,7 +9062,7 @@
       <c r="R67" s="18"/>
       <c r="S67" s="7"/>
     </row>
-    <row r="68" spans="1:19">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>216</v>
       </c>
@@ -9094,7 +9103,7 @@
       <c r="R68" s="18"/>
       <c r="S68" s="7"/>
     </row>
-    <row r="69" spans="1:19">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>170</v>
       </c>
@@ -9139,7 +9148,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="70" spans="1:19">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>245</v>
       </c>
@@ -9184,7 +9193,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="71" spans="1:19">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>193</v>
       </c>
@@ -9229,7 +9238,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="72" spans="1:19">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>178</v>
       </c>
@@ -9276,7 +9285,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="73" spans="1:19">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>24</v>
       </c>
@@ -9321,7 +9330,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="74" spans="1:19">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>197</v>
       </c>
@@ -9362,7 +9371,7 @@
       <c r="R74" s="20"/>
       <c r="S74" s="7"/>
     </row>
-    <row r="75" spans="1:19">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>161</v>
       </c>
@@ -9403,7 +9412,7 @@
       <c r="R75" s="20"/>
       <c r="S75" s="7"/>
     </row>
-    <row r="76" spans="1:19">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>182</v>
       </c>
@@ -9444,7 +9453,7 @@
       <c r="R76" s="20"/>
       <c r="S76" s="7"/>
     </row>
-    <row r="77" spans="1:19">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>201</v>
       </c>
@@ -9485,7 +9494,7 @@
       <c r="R77" s="20"/>
       <c r="S77" s="7"/>
     </row>
-    <row r="78" spans="1:19">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>19</v>
       </c>
@@ -9526,7 +9535,7 @@
       <c r="R78" s="20"/>
       <c r="S78" s="7"/>
     </row>
-    <row r="79" spans="1:19">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>225</v>
       </c>
@@ -9567,7 +9576,7 @@
       <c r="R79" s="20"/>
       <c r="S79" s="7"/>
     </row>
-    <row r="80" spans="1:19">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>205</v>
       </c>
@@ -9608,7 +9617,7 @@
       <c r="R80" s="20"/>
       <c r="S80" s="7"/>
     </row>
-    <row r="86" spans="1:21">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>210</v>
       </c>

</xml_diff>